<commit_message>
added Navicent Health Baldwin
</commit_message>
<xml_diff>
--- a/AirComm.xlsx
+++ b/AirComm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthammond/Documents/Maps/AUG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A47B6DF-B3FD-814B-AAF6-A433ED450920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84EAF11A-860F-D848-A1F2-529E0EDDB849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{9EF95D2B-8697-FD42-ADB2-522E985180DE}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="463">
   <si>
     <t>FAA IDENTIFIER</t>
   </si>
@@ -1411,6 +1411,18 @@
   </si>
   <si>
     <t>Effingham Hosp-Springfield, GA</t>
+  </si>
+  <si>
+    <t>33 05.39 N</t>
+  </si>
+  <si>
+    <t>83 14.63 W</t>
+  </si>
+  <si>
+    <t>NAVIC</t>
+  </si>
+  <si>
+    <t>Navicent Health Baldwin-Milledgeville, GA</t>
   </si>
 </sst>
 </file>
@@ -1881,8 +1893,8 @@
   <dimension ref="A1:F998"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2941,96 +2953,96 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="13" t="s">
-        <v>165</v>
+        <v>459</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>166</v>
+        <v>460</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>163</v>
+        <v>461</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="E53" s="13" t="s">
-        <v>164</v>
-      </c>
+        <v>462</v>
+      </c>
+      <c r="E53" s="13"/>
       <c r="F53" s="9" t="str">
         <f>IF(E53&lt;&gt;"","YES","NO")</f>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="13" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="E54" s="13"/>
+        <v>377</v>
+      </c>
+      <c r="E54" s="13" t="s">
+        <v>164</v>
+      </c>
       <c r="F54" s="9" t="str">
         <f>IF(E54&lt;&gt;"","YES","NO")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="B55" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="C55" s="18" t="s">
-        <v>173</v>
-      </c>
-      <c r="D55" t="s">
-        <v>380</v>
-      </c>
-      <c r="E55" s="14" t="s">
-        <v>174</v>
-      </c>
+      <c r="A55" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="C55" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="E55" s="13"/>
       <c r="F55" s="9" t="str">
         <f>IF(E55&lt;&gt;"","YES","NO")</f>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="B56" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="C56" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>379</v>
-      </c>
-      <c r="E56" s="13"/>
+      <c r="A56" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="D56" t="s">
+        <v>380</v>
+      </c>
+      <c r="E56" s="14" t="s">
+        <v>174</v>
+      </c>
       <c r="F56" s="9" t="str">
         <f>IF(E56&lt;&gt;"","YES","NO")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="13" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E57" s="13"/>
       <c r="F57" s="9" t="str">
@@ -3040,40 +3052,38 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="13" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="E58" s="13" t="s">
-        <v>181</v>
-      </c>
+        <v>381</v>
+      </c>
+      <c r="E58" s="13"/>
       <c r="F58" s="9" t="str">
         <f>IF(E58&lt;&gt;"","YES","NO")</f>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="13" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E59" s="13" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="F59" s="9" t="str">
         <f>IF(E59&lt;&gt;"","YES","NO")</f>
@@ -3082,19 +3092,19 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="13" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E60" s="13" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="F60" s="9" t="str">
         <f>IF(E60&lt;&gt;"","YES","NO")</f>
@@ -3103,19 +3113,19 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="13" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E61" s="13" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F61" s="9" t="str">
         <f>IF(E61&lt;&gt;"","YES","NO")</f>
@@ -3124,59 +3134,59 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="13" t="s">
-        <v>430</v>
+        <v>194</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>431</v>
+        <v>195</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>432</v>
+        <v>192</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>433</v>
-      </c>
-      <c r="E62" s="13"/>
+        <v>385</v>
+      </c>
+      <c r="E62" s="13" t="s">
+        <v>193</v>
+      </c>
       <c r="F62" s="9" t="str">
         <f>IF(E62&lt;&gt;"","YES","NO")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="13" t="s">
-        <v>198</v>
+        <v>430</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>199</v>
+        <v>431</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>196</v>
+        <v>432</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="E63" s="13" t="s">
-        <v>197</v>
-      </c>
+        <v>433</v>
+      </c>
+      <c r="E63" s="13"/>
       <c r="F63" s="9" t="str">
         <f>IF(E63&lt;&gt;"","YES","NO")</f>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="13" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E64" s="13" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F64" s="9" t="str">
         <f>IF(E64&lt;&gt;"","YES","NO")</f>
@@ -3185,35 +3195,37 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="13" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="E65" s="13"/>
+        <v>387</v>
+      </c>
+      <c r="E65" s="13" t="s">
+        <v>201</v>
+      </c>
       <c r="F65" s="9" t="str">
         <f>IF(E65&lt;&gt;"","YES","NO")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="13" t="s">
-        <v>322</v>
+        <v>205</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>323</v>
+        <v>206</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>321</v>
+        <v>204</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E66" s="13"/>
       <c r="F66" s="9" t="str">
@@ -3223,77 +3235,77 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="13" t="s">
-        <v>209</v>
+        <v>322</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>210</v>
+        <v>323</v>
       </c>
       <c r="C67" s="17" t="s">
-        <v>207</v>
+        <v>321</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>390</v>
-      </c>
-      <c r="E67" s="13" t="s">
-        <v>208</v>
-      </c>
+        <v>389</v>
+      </c>
+      <c r="E67" s="13"/>
       <c r="F67" s="9" t="str">
         <f>IF(E67&lt;&gt;"","YES","NO")</f>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="13" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C68" s="17" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>391</v>
-      </c>
-      <c r="E68" s="13"/>
+        <v>390</v>
+      </c>
+      <c r="E68" s="13" t="s">
+        <v>208</v>
+      </c>
       <c r="F68" s="9" t="str">
         <f>IF(E68&lt;&gt;"","YES","NO")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="14" t="s">
-        <v>448</v>
-      </c>
-      <c r="B69" s="14" t="s">
-        <v>449</v>
-      </c>
-      <c r="C69" s="18" t="s">
-        <v>450</v>
+      <c r="A69" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="B69" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="C69" s="17" t="s">
+        <v>211</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>447</v>
-      </c>
-      <c r="E69" s="14"/>
+        <v>391</v>
+      </c>
+      <c r="E69" s="13"/>
       <c r="F69" s="9" t="str">
         <f>IF(E69&lt;&gt;"","YES","NO")</f>
         <v>NO</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="B70" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="C70" s="17" t="s">
-        <v>214</v>
+      <c r="A70" s="14" t="s">
+        <v>448</v>
+      </c>
+      <c r="B70" s="14" t="s">
+        <v>449</v>
+      </c>
+      <c r="C70" s="18" t="s">
+        <v>450</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>392</v>
-      </c>
-      <c r="E70" s="13"/>
+        <v>447</v>
+      </c>
+      <c r="E70" s="14"/>
       <c r="F70" s="9" t="str">
         <f>IF(E70&lt;&gt;"","YES","NO")</f>
         <v>NO</v>
@@ -3301,80 +3313,78 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="13" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C71" s="17" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="E71" s="13" t="s">
-        <v>218</v>
-      </c>
+        <v>392</v>
+      </c>
+      <c r="E71" s="13"/>
       <c r="F71" s="9" t="str">
         <f>IF(E71&lt;&gt;"","YES","NO")</f>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="13" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C72" s="17" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>394</v>
-      </c>
-      <c r="E72" s="13"/>
+        <v>393</v>
+      </c>
+      <c r="E72" s="13" t="s">
+        <v>218</v>
+      </c>
       <c r="F72" s="9" t="str">
         <f>IF(E72&lt;&gt;"","YES","NO")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="13" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C73" s="17" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>395</v>
-      </c>
-      <c r="E73" s="13" t="s">
-        <v>225</v>
-      </c>
+        <v>394</v>
+      </c>
+      <c r="E73" s="13"/>
       <c r="F73" s="9" t="str">
         <f>IF(E73&lt;&gt;"","YES","NO")</f>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="13" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C74" s="17" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E74" s="13" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="F74" s="9" t="str">
         <f>IF(E74&lt;&gt;"","YES","NO")</f>
@@ -3383,19 +3393,19 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="13" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C75" s="17" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E75" s="13" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="F75" s="9" t="str">
         <f>IF(E75&lt;&gt;"","YES","NO")</f>
@@ -3404,19 +3414,19 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="13" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C76" s="17" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E76" s="13" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F76" s="9" t="str">
         <f>IF(E76&lt;&gt;"","YES","NO")</f>
@@ -3425,19 +3435,19 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="13" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C77" s="17" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E77" s="13" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F77" s="9" t="str">
         <f>IF(E77&lt;&gt;"","YES","NO")</f>
@@ -3446,19 +3456,19 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="13" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C78" s="17" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E78" s="13" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F78" s="9" t="str">
         <f>IF(E78&lt;&gt;"","YES","NO")</f>
@@ -3467,59 +3477,59 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="13" t="s">
-        <v>426</v>
+        <v>246</v>
       </c>
       <c r="B79" s="13" t="s">
-        <v>427</v>
+        <v>247</v>
       </c>
       <c r="C79" s="17" t="s">
-        <v>428</v>
+        <v>244</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>429</v>
-      </c>
-      <c r="E79" s="13"/>
+        <v>400</v>
+      </c>
+      <c r="E79" s="13" t="s">
+        <v>245</v>
+      </c>
       <c r="F79" s="9" t="str">
         <f>IF(E79&lt;&gt;"","YES","NO")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="13" t="s">
-        <v>250</v>
+        <v>426</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>251</v>
+        <v>427</v>
       </c>
       <c r="C80" s="17" t="s">
-        <v>248</v>
+        <v>428</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>401</v>
-      </c>
-      <c r="E80" s="13" t="s">
-        <v>249</v>
-      </c>
+        <v>429</v>
+      </c>
+      <c r="E80" s="13"/>
       <c r="F80" s="9" t="str">
         <f>IF(E80&lt;&gt;"","YES","NO")</f>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="13" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C81" s="17" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E81" s="13" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="F81" s="9" t="str">
         <f>IF(E81&lt;&gt;"","YES","NO")</f>
@@ -3528,19 +3538,19 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="13" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C82" s="17" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E82" s="13" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F82" s="9" t="str">
         <f>IF(E82&lt;&gt;"","YES","NO")</f>
@@ -3549,19 +3559,19 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="13" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B83" s="13" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C83" s="17" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E83" s="13" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="F83" s="9" t="str">
         <f>IF(E83&lt;&gt;"","YES","NO")</f>
@@ -3570,75 +3580,77 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="13" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B84" s="13" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C84" s="17" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>405</v>
-      </c>
-      <c r="E84" s="13"/>
+        <v>404</v>
+      </c>
+      <c r="E84" s="13" t="s">
+        <v>261</v>
+      </c>
       <c r="F84" s="9" t="str">
         <f>IF(E84&lt;&gt;"","YES","NO")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="13" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B85" s="13" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C85" s="17" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="E85" s="13" t="s">
-        <v>268</v>
-      </c>
+        <v>405</v>
+      </c>
+      <c r="E85" s="13"/>
       <c r="F85" s="9" t="str">
         <f>IF(E85&lt;&gt;"","YES","NO")</f>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="13" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B86" s="13" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C86" s="17" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>407</v>
-      </c>
-      <c r="E86" s="13"/>
+        <v>406</v>
+      </c>
+      <c r="E86" s="13" t="s">
+        <v>268</v>
+      </c>
       <c r="F86" s="9" t="str">
         <f>IF(E86&lt;&gt;"","YES","NO")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="13" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B87" s="13" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C87" s="17" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E87" s="13"/>
       <c r="F87" s="9" t="str">
@@ -3647,41 +3659,39 @@
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88" s="14" t="s">
-        <v>282</v>
-      </c>
-      <c r="B88" s="14" t="s">
-        <v>283</v>
-      </c>
-      <c r="C88" s="18" t="s">
-        <v>434</v>
-      </c>
-      <c r="D88" t="s">
-        <v>410</v>
-      </c>
-      <c r="E88" s="14" t="s">
-        <v>281</v>
-      </c>
+      <c r="A88" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="B88" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="C88" s="17" t="s">
+        <v>274</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="E88" s="13"/>
       <c r="F88" s="9" t="str">
         <f>IF(E88&lt;&gt;"","YES","NO")</f>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" s="13" t="s">
-        <v>279</v>
-      </c>
-      <c r="B89" s="13" t="s">
-        <v>280</v>
-      </c>
-      <c r="C89" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="D89" s="5" t="s">
-        <v>409</v>
-      </c>
-      <c r="E89" s="13" t="s">
-        <v>278</v>
+      <c r="A89" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="B89" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="C89" s="18" t="s">
+        <v>434</v>
+      </c>
+      <c r="D89" t="s">
+        <v>410</v>
+      </c>
+      <c r="E89" s="14" t="s">
+        <v>281</v>
       </c>
       <c r="F89" s="9" t="str">
         <f>IF(E89&lt;&gt;"","YES","NO")</f>
@@ -3690,99 +3700,99 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="13" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="B90" s="13" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="C90" s="17" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>411</v>
-      </c>
-      <c r="E90" s="13"/>
+        <v>409</v>
+      </c>
+      <c r="E90" s="13" t="s">
+        <v>278</v>
+      </c>
       <c r="F90" s="9" t="str">
         <f>IF(E90&lt;&gt;"","YES","NO")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="13" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B91" s="13" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C91" s="17" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>412</v>
-      </c>
-      <c r="E91" s="13" t="s">
-        <v>288</v>
-      </c>
+        <v>411</v>
+      </c>
+      <c r="E91" s="13"/>
       <c r="F91" s="9" t="str">
         <f>IF(E91&lt;&gt;"","YES","NO")</f>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="13" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B92" s="13" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C92" s="17" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>413</v>
-      </c>
-      <c r="E92" s="13"/>
+        <v>412</v>
+      </c>
+      <c r="E92" s="13" t="s">
+        <v>288</v>
+      </c>
       <c r="F92" s="9" t="str">
         <f>IF(E92&lt;&gt;"","YES","NO")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="13" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B93" s="13" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C93" s="17" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>414</v>
-      </c>
-      <c r="E93" s="13" t="s">
-        <v>295</v>
-      </c>
+        <v>413</v>
+      </c>
+      <c r="E93" s="13"/>
       <c r="F93" s="9" t="str">
         <f>IF(E93&lt;&gt;"","YES","NO")</f>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="13" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="B94" s="13" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="C94" s="17" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E94" s="13" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="F94" s="9" t="str">
         <f>IF(E94&lt;&gt;"","YES","NO")</f>
@@ -3791,59 +3801,59 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="13" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="B95" s="13" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="C95" s="17" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>415</v>
-      </c>
-      <c r="E95" s="13"/>
+        <v>416</v>
+      </c>
+      <c r="E95" s="13" t="s">
+        <v>302</v>
+      </c>
       <c r="F95" s="9" t="str">
         <f>IF(E95&lt;&gt;"","YES","NO")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="13" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="B96" s="13" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="C96" s="17" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>417</v>
-      </c>
-      <c r="E96" s="13" t="s">
-        <v>306</v>
-      </c>
+        <v>415</v>
+      </c>
+      <c r="E96" s="13"/>
       <c r="F96" s="9" t="str">
         <f>IF(E96&lt;&gt;"","YES","NO")</f>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="13" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B97" s="13" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C97" s="17" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E97" s="13" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F97" s="9" t="str">
         <f>IF(E97&lt;&gt;"","YES","NO")</f>
@@ -3852,19 +3862,19 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="13" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B98" s="13" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C98" s="17" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E98" s="13" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="F98" s="9" t="str">
         <f>IF(E98&lt;&gt;"","YES","NO")</f>
@@ -3873,19 +3883,19 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="13" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B99" s="13" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C99" s="17" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E99" s="13" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="F99" s="9" t="str">
         <f>IF(E99&lt;&gt;"","YES","NO")</f>
@@ -3894,30 +3904,43 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="13" t="s">
-        <v>435</v>
+        <v>319</v>
       </c>
       <c r="B100" s="13" t="s">
-        <v>436</v>
+        <v>320</v>
       </c>
       <c r="C100" s="17" t="s">
-        <v>437</v>
+        <v>317</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>442</v>
-      </c>
-      <c r="E100" s="13"/>
+        <v>420</v>
+      </c>
+      <c r="E100" s="13" t="s">
+        <v>318</v>
+      </c>
       <c r="F100" s="9" t="str">
         <f>IF(E100&lt;&gt;"","YES","NO")</f>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" s="13" t="s">
+        <v>435</v>
+      </c>
+      <c r="B101" s="13" t="s">
+        <v>436</v>
+      </c>
+      <c r="C101" s="17" t="s">
+        <v>437</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="E101" s="13"/>
+      <c r="F101" s="9" t="str">
+        <f>IF(E101&lt;&gt;"","YES","NO")</f>
         <v>NO</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A101" s="13"/>
-      <c r="B101" s="13"/>
-      <c r="C101" s="17"/>
-      <c r="D101" s="5"/>
-      <c r="E101" s="13"/>
-      <c r="F101" s="9"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="13"/>
@@ -11096,8 +11119,8 @@
       <c r="F998" s="10"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F100">
-    <sortCondition ref="D2:D100"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F101">
+    <sortCondition ref="D2:D101"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>